<commit_message>
Leicht angepasst nach Kassel und Darmstadt
</commit_message>
<xml_diff>
--- a/index/obwahl_ks_2023/kandidaten.xlsx
+++ b/index/obwahl_ks_2023/kandidaten.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Dr. Sven</t>
   </si>
   <si>
-    <t xml:space="preserve">Schöller</t>
+    <t xml:space="preserve">Schoeller</t>
   </si>
   <si>
     <t xml:space="preserve">Grüne</t>
@@ -263,7 +263,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>